<commit_message>
SP para importar tarifas varias con cambios en las tablas
</commit_message>
<xml_diff>
--- a/dataImport/Datos socios.xlsx
+++ b/dataImport/Datos socios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lautaro_Santillan\UNLaM\Bases de Datos Aplicada\SolNorte-Grupo3-BDDA\SOLNORTE-GRUPO3-BDDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lautaro_Santillan\UNLaM\Bases de Datos Aplicada\SolNorte-Grupo3-BDDA\SOLNORTE-GRUPO3-BDDA\dataImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA42708E-501B-4C86-BCFA-11F87F12CA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4983A4B-2A06-4916-A40B-1711484823EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="3765" windowWidth="17280" windowHeight="9420" tabRatio="732" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2496" yWindow="1908" windowWidth="17280" windowHeight="9420" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables de Pago" sheetId="1" r:id="rId1"/>
@@ -32444,7 +32444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E70FEA9-2699-4D25-8C16-D7DDE65501C1}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -32695,7 +32695,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I928"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
@@ -49199,6 +49199,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0244CD539E758458F9751B276EDBDB5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b8b8c40857de5fa74dc501c9010f9b13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29" xmlns:ns3="5ab81898-6d95-4a49-9528-d5d2a870eede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba6727053a82ee7f0bb58b7bd192b345" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
@@ -49409,26 +49428,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F9A25F6-D4B8-4181-A5F5-CE5E6C4D6717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="5ab81898-6d95-4a49-9528-d5d2a870eede"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B3BBDB-C708-4BF2-AF52-39E7216A2396}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0048A681-FC7F-4BB5-868D-AE844DB2E4E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -49445,29 +49470,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B3BBDB-C708-4BF2-AF52-39E7216A2396}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F9A25F6-D4B8-4181-A5F5-CE5E6C4D6717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="5ab81898-6d95-4a49-9528-d5d2a870eede"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
SP para importar grupos familiares
</commit_message>
<xml_diff>
--- a/dataImport/Datos socios.xlsx
+++ b/dataImport/Datos socios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lautaro_Santillan\UNLaM\Bases de Datos Aplicada\SolNorte-Grupo3-BDDA\SOLNORTE-GRUPO3-BDDA\dataImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4983A4B-2A06-4916-A40B-1711484823EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3FFEC-EFE2-4E7D-8C34-7F9BDEF5048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="1908" windowWidth="17280" windowHeight="9420" tabRatio="732" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="732" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Responsables de Pago" sheetId="1" r:id="rId1"/>
@@ -2268,16 +2268,7 @@
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6821,11 +6812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081E0048-651A-4FD8-A0B0-945A4642362D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A20"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6882,7 +6872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>560</v>
       </c>
@@ -6970,7 +6960,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>561</v>
       </c>
@@ -7004,7 +6994,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>562</v>
       </c>
@@ -7038,7 +7028,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>563</v>
       </c>
@@ -7096,7 +7086,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>564</v>
       </c>
@@ -7130,7 +7120,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>565</v>
       </c>
@@ -7164,7 +7154,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>566</v>
       </c>
@@ -7192,7 +7182,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>567</v>
       </c>
@@ -7292,7 +7282,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>569</v>
       </c>
@@ -7324,7 +7314,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>570</v>
       </c>
@@ -7480,7 +7470,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>574</v>
       </c>
@@ -7512,7 +7502,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>575</v>
       </c>
@@ -7633,7 +7623,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>635</v>
       </c>
@@ -7786,7 +7776,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>637</v>
       </c>
@@ -7903,11 +7893,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G35" xr:uid="{081E0048-651A-4FD8-A0B0-945A4642362D}">
-    <filterColumn colId="6">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G35" xr:uid="{081E0048-651A-4FD8-A0B0-945A4642362D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L35">
     <sortCondition ref="B2:B35"/>
   </sortState>
@@ -32444,7 +32430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E70FEA9-2699-4D25-8C16-D7DDE65501C1}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -49199,25 +49185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0244CD539E758458F9751B276EDBDB5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b8b8c40857de5fa74dc501c9010f9b13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29" xmlns:ns3="5ab81898-6d95-4a49-9528-d5d2a870eede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba6727053a82ee7f0bb58b7bd192b345" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
@@ -49428,32 +49395,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F9A25F6-D4B8-4181-A5F5-CE5E6C4D6717}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="5ab81898-6d95-4a49-9528-d5d2a870eede"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B3BBDB-C708-4BF2-AF52-39E7216A2396}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0048A681-FC7F-4BB5-868D-AE844DB2E4E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -49470,4 +49431,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B3BBDB-C708-4BF2-AF52-39E7216A2396}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F9A25F6-D4B8-4181-A5F5-CE5E6C4D6717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="5ab81898-6d95-4a49-9528-d5d2a870eede"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>